<commit_message>
some qol and add StateDebugger.
</commit_message>
<xml_diff>
--- a/Tools/Luban/Datas/Mobs.xlsx
+++ b/Tools/Luban/Datas/Mobs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30217C7-1A29-4FE9-99AA-090FD7589EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5977FB0-28B5-4740-8B6D-E53B65DCE659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mobs" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
   <si>
     <t>##var</t>
   </si>
@@ -169,10 +169,6 @@
   </si>
   <si>
     <t>targeting</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>转向速度</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -649,10 +645,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D1:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -706,16 +702,16 @@
         <v>18</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -829,22 +825,22 @@
         <v>16</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -3436,22 +3432,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0701E0-B242-4436-8224-C8C9DE09C2EB}">
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14" style="9" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="9" customWidth="1"/>
-    <col min="6" max="8" width="12.5546875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" style="9" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" style="9" customWidth="1"/>
-    <col min="11" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5546875" customWidth="1"/>
     <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
@@ -3487,10 +3486,18 @@
       <c r="I1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
+      <c r="J1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -3530,10 +3537,18 @@
       <c r="I2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="J2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -3595,15 +3610,23 @@
         <v>16</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
+      <c r="J4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -3621,10 +3644,10 @@
         <v>1001</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="4">
         <v>400</v>
@@ -3641,10 +3664,18 @@
       <c r="I5" s="4">
         <v>0.1</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
+      <c r="J5" s="4">
+        <v>4</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
+        <v>5</v>
+      </c>
+      <c r="M5" s="3">
+        <v>10</v>
+      </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>

</xml_diff>

<commit_message>
The Knight 只剩 音效
</commit_message>
<xml_diff>
--- a/Tools/Luban/Datas/Mobs.xlsx
+++ b/Tools/Luban/Datas/Mobs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57AF4EE-7150-4844-B014-3331CFAE1E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD12B87-A803-4B8A-B039-AA3873FFB9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12561" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3449,7 +3449,7 @@
   <dimension ref="A1:W100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -3603,7 +3603,7 @@
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
     </row>
-    <row r="4" spans="1:23" ht="36.299999999999997" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -3770,10 +3770,10 @@
         <v>300</v>
       </c>
       <c r="G7" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H7" s="4">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="I7" s="4">
         <v>0.1</v>

</xml_diff>